<commit_message>
add graphical interface for data modification
</commit_message>
<xml_diff>
--- a/python_version/DataTest/test.xlsx
+++ b/python_version/DataTest/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Projets\musicocktails\GIT\musicocktail\python_version\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Projets\musicocktails\GIT\musicocktail\python_version\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC93D9F-263D-497B-9DB8-7E2B6E483757}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D21711-4894-4A97-AF69-3FEFEFFE1F8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recettes" sheetId="1" r:id="rId1"/>
@@ -1878,9 +1878,6 @@
     <t>Flavors</t>
   </si>
   <si>
-    <t>Clarke_broke</t>
-  </si>
-  <si>
     <t>Gary_Regan</t>
   </si>
   <si>
@@ -1912,6 +1909,9 @@
   </si>
   <si>
     <t>author</t>
+  </si>
+  <si>
+    <t>Paul_Clarke</t>
   </si>
 </sst>
 </file>
@@ -2341,8 +2341,8 @@
   </sheetPr>
   <dimension ref="A1:FB539"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AT6" sqref="AT6"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -2484,22 +2484,22 @@
         <v>613</v>
       </c>
       <c r="AN1" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="AO1" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>618</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>619</v>
       </c>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -18546,7 +18546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -18560,10 +18560,10 @@
         <v>160</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>624</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>625</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>161</v>
@@ -18577,20 +18577,20 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E2">
         <v>1723</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>